<commit_message>
Adiciona a criação de itop para pedido de permissões
</commit_message>
<xml_diff>
--- a/fichas/Ficha IT.xlsx
+++ b/fichas/Ficha IT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Machado\Dropbox\Pessoal\Formação\Escolas_fisicas\IPL\Mestrado\Business Analytics\Projeto\criar-acessos\fichas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CDB331-1B80-4B41-B6EE-C473C7D5BBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB5972B-E406-4A0D-BFF3-AC1B612A637E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>Informações do Colaborador</t>
   </si>
@@ -664,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -726,37 +726,37 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -768,35 +768,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -804,28 +790,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
@@ -856,22 +820,61 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1303,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,12 +1325,12 @@
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1379,21 +1382,21 @@
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="68"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32"/>
@@ -1411,32 +1414,36 @@
       <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="6" t="s">
         <v>62</v>
       </c>
@@ -1446,32 +1453,36 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="6"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="33" t="s">
@@ -1481,37 +1492,37 @@
       <c r="G23" s="34"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="60"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="36"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="40"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="62"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="32"/>
@@ -1529,10 +1540,10 @@
       <c r="G29" s="34"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="22"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
@@ -1540,10 +1551,10 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="22"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
@@ -1551,10 +1562,10 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="22"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
@@ -1562,10 +1573,10 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="22"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
@@ -1573,10 +1584,10 @@
       <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="22"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
@@ -1587,18 +1598,18 @@
       <c r="A35" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="42"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="25"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="43"/>
-      <c r="B36" s="44"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="5" t="s">
         <v>11</v>
       </c>
@@ -1610,84 +1621,84 @@
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="22"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="45" t="s">
+      <c r="E37" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="45"/>
-      <c r="G37" s="46"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="42"/>
     </row>
     <row r="38" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="22"/>
+      <c r="B38" s="23"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="45" t="s">
+      <c r="E38" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="45"/>
-      <c r="G38" s="46"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="42"/>
     </row>
     <row r="39" spans="1:7" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="22"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="45" t="s">
+      <c r="E39" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="45"/>
-      <c r="G39" s="46"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="42"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="22"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="45" t="s">
+      <c r="E40" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F40" s="45"/>
-      <c r="G40" s="46"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="42"/>
     </row>
     <row r="41" spans="1:7" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="50"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="56"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="51" t="s">
+      <c r="A43" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="52"/>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="43"/>
-      <c r="B44" s="44"/>
+      <c r="A44" s="28"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="9" t="s">
         <v>11</v>
       </c>
@@ -1701,10 +1712,10 @@
       <c r="G44" s="34"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5"/>
@@ -1712,10 +1723,10 @@
       <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="22"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="5"/>
@@ -1723,10 +1734,10 @@
       <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="22"/>
+      <c r="B47" s="23"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="5"/>
@@ -1743,8 +1754,8 @@
       <c r="G48" s="12"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="43"/>
-      <c r="B49" s="44"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="29"/>
       <c r="C49" s="5" t="s">
         <v>11</v>
       </c>
@@ -1758,10 +1769,10 @@
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="21" t="s">
+      <c r="A50" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="22"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
@@ -1769,10 +1780,10 @@
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="48"/>
+      <c r="B51" s="40"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="33"/>
@@ -1780,67 +1791,67 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="1:7" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="48"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="45" t="s">
+      <c r="E52" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="F52" s="45"/>
-      <c r="G52" s="46"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="42"/>
     </row>
     <row r="53" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="48"/>
+      <c r="B53" s="40"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
-      <c r="E53" s="45" t="s">
+      <c r="E53" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F53" s="45"/>
-      <c r="G53" s="46"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="42"/>
     </row>
     <row r="54" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="55" t="s">
+      <c r="A54" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="56"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="59"/>
-      <c r="E54" s="61" t="s">
+      <c r="B54" s="44"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="F54" s="61"/>
-      <c r="G54" s="62"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="50"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="57"/>
-      <c r="B55" s="58"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="63" t="s">
+      <c r="A55" s="45"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="F55" s="63"/>
-      <c r="G55" s="64"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="52"/>
     </row>
     <row r="56" spans="1:7" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="42"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="25"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="13"/>
@@ -1852,8 +1863,8 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="43"/>
-      <c r="B58" s="44"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="9" t="s">
         <v>11</v>
       </c>
@@ -1867,10 +1878,10 @@
       <c r="G58" s="34"/>
     </row>
     <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="22"/>
+      <c r="B59" s="23"/>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
       <c r="E59" s="5"/>
@@ -1878,8 +1889,8 @@
       <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="21"/>
-      <c r="B60" s="22"/>
+      <c r="A60" s="22"/>
+      <c r="B60" s="23"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
       <c r="E60" s="5"/>
@@ -1890,14 +1901,14 @@
       <c r="A61" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="65" t="s">
+      <c r="B61" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="65"/>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65"/>
-      <c r="F61" s="65"/>
-      <c r="G61" s="66"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="36"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="13"/>
@@ -1930,10 +1941,10 @@
       <c r="G65" s="34"/>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="21" t="s">
+      <c r="A66" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B66" s="22"/>
+      <c r="B66" s="23"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
@@ -1941,10 +1952,10 @@
       <c r="G66" s="7"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B67" s="22"/>
+      <c r="B67" s="23"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="5"/>
@@ -1952,8 +1963,8 @@
       <c r="G67" s="7"/>
     </row>
     <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="43"/>
-      <c r="B68" s="44"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="29"/>
       <c r="C68" s="16"/>
       <c r="D68" s="16"/>
       <c r="E68" s="15"/>
@@ -1961,10 +1972,10 @@
       <c r="G68" s="17"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="21" t="s">
+      <c r="A69" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B69" s="22"/>
+      <c r="B69" s="23"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
@@ -1972,8 +1983,8 @@
       <c r="G69" s="7"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="43"/>
-      <c r="B70" s="44"/>
+      <c r="A70" s="28"/>
+      <c r="B70" s="29"/>
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
@@ -1984,12 +1995,12 @@
       <c r="A71" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="69"/>
-      <c r="C71" s="69"/>
-      <c r="D71" s="69"/>
-      <c r="E71" s="69"/>
-      <c r="F71" s="69"/>
-      <c r="G71" s="70"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="31"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
@@ -2022,10 +2033,10 @@
       <c r="G75" s="34"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="21" t="s">
+      <c r="A76" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B76" s="22"/>
+      <c r="B76" s="23"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -2033,10 +2044,10 @@
       <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="21" t="s">
+      <c r="A77" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B77" s="22"/>
+      <c r="B77" s="23"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -2047,14 +2058,14 @@
       <c r="A78" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B78" s="41" t="s">
+      <c r="B78" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C78" s="41"/>
-      <c r="D78" s="41"/>
-      <c r="E78" s="41"/>
-      <c r="F78" s="41"/>
-      <c r="G78" s="42"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="25"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
@@ -2075,10 +2086,10 @@
       <c r="A82" s="8"/>
     </row>
     <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="67" t="s">
+      <c r="A83" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B83" s="68"/>
+      <c r="B83" s="27"/>
     </row>
     <row r="84" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="18" t="s">
@@ -2090,20 +2101,50 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="B78:G78"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="B61:G61"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:G25"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="B56:G56"/>
     <mergeCell ref="A43:G43"/>
@@ -2120,50 +2161,20 @@
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="E54:G54"/>
     <mergeCell ref="E55:G55"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:G25"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B61:G61"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="B78:G78"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="A76:B76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>